<commit_message>
Doan day template 12/04/2019
</commit_message>
<xml_diff>
--- a/2.Design/Template/Thong_tin_chitiet_giao_dich.xlsx
+++ b/2.Design/Template/Thong_tin_chitiet_giao_dich.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WMS\temp\file_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2.DoanLV4_Document\LogDez\1.Document\WMS_Documents\2.Design\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00903929-AA93-4157-BB20-10199A733F9D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BBE379-73AC-4835-9E39-6F0339F6E721}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -258,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -299,19 +299,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -630,7 +627,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -639,56 +636,59 @@
     <col min="2" max="2" width="19.1796875" style="5" customWidth="1"/>
     <col min="3" max="3" width="20.90625" style="5" customWidth="1"/>
     <col min="4" max="6" width="9.7265625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.54296875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="30.7265625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="11.7265625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="9.7265625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="9.08984375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="10.54296875" style="5" customWidth="1"/>
-    <col min="15" max="15" width="10.6328125" style="5" customWidth="1"/>
-    <col min="16" max="16" width="10.08984375" customWidth="1"/>
-    <col min="17" max="17" width="13.54296875" customWidth="1"/>
+    <col min="7" max="7" width="10.6328125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="30.7265625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="11.7265625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="9.7265625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="9.08984375" style="5" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="10.54296875" style="5" customWidth="1"/>
+    <col min="16" max="16" width="10.6328125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="10.08984375" customWidth="1"/>
+    <col min="18" max="18" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
       <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
     </row>
     <row r="3" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -709,38 +709,38 @@
       <c r="F3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="M3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="N3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="O3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="P3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="Q3" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -752,17 +752,17 @@
       <c r="D4" s="2"/>
       <c r="E4" s="1"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="2"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="3"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="15"/>
     </row>
     <row r="5" spans="1:17" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -783,38 +783,38 @@
       <c r="F5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="K5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="M5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="N5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -826,22 +826,22 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="3"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>